<commit_message>
Extended functionality in instance generator
</commit_message>
<xml_diff>
--- a/input/orders.xlsx
+++ b/input/orders.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andersvandvik/Repositories/project-thesis/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E36713A-93A8-164E-846B-FAB8E67D95F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8038BF-619A-A345-9164-A12437329461}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{9863645F-DB31-A24D-8693-F81557060D8C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{9863645F-DB31-A24D-8693-F81557060D8C}"/>
   </bookViews>
   <sheets>
     <sheet name="CS-I2" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="CS-I3" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>SEQ</t>
+  </si>
+  <si>
+    <t>TRO</t>
+  </si>
+  <si>
+    <t>OP</t>
   </si>
 </sst>
 </file>
@@ -419,7 +425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D185F467-10F0-394B-B6C9-1EF394BB90DE}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
@@ -488,12 +494,99 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E02BCBB6-69BF-5844-97F7-F0617359B90D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Saving data from run
</commit_message>
<xml_diff>
--- a/input/orders.xlsx
+++ b/input/orders.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andersvandvik/Repositories/project-thesis/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8038BF-619A-A345-9164-A12437329461}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26617500-087D-F847-89EA-C1E9B790C1E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{9863645F-DB31-A24D-8693-F81557060D8C}"/>
   </bookViews>
   <sheets>
-    <sheet name="CS-I2" sheetId="1" r:id="rId1"/>
-    <sheet name="CS-I3" sheetId="2" r:id="rId2"/>
+    <sheet name="C-I2" sheetId="1" r:id="rId1"/>
+    <sheet name="C-I3" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -497,7 +497,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>